<commit_message>
correct sku model map
</commit_message>
<xml_diff>
--- a/results/rmse_all_preds_jan_17.xlsx
+++ b/results/rmse_all_preds_jan_17.xlsx
@@ -1258,10 +1258,10 @@
         <v>3.100806346742731</v>
       </c>
       <c r="AJ7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="AK7" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:37">
@@ -1805,10 +1805,10 @@
         <v>1.177618662507399</v>
       </c>
       <c r="AJ12">
+        <v>2</v>
+      </c>
+      <c r="AK12" t="s">
         <v>6</v>
-      </c>
-      <c r="AK12" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:37">
@@ -3595,10 +3595,10 @@
         <v>1.362770287738494</v>
       </c>
       <c r="AJ28">
+        <v>2</v>
+      </c>
+      <c r="AK28" t="s">
         <v>6</v>
-      </c>
-      <c r="AK28" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="29" spans="1:37">
@@ -4255,10 +4255,10 @@
         <v>0.7176350047203662</v>
       </c>
       <c r="AJ34">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="AK34" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="35" spans="1:37">
@@ -5593,10 +5593,10 @@
         <v>1.863272850198197</v>
       </c>
       <c r="AJ46">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="AK46" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
     </row>
     <row r="47" spans="1:37">
@@ -8852,10 +8852,10 @@
         <v>0.7842193570679061</v>
       </c>
       <c r="AJ75">
+        <v>2</v>
+      </c>
+      <c r="AK75" t="s">
         <v>6</v>
-      </c>
-      <c r="AK75" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="76" spans="1:37">
@@ -10303,10 +10303,10 @@
         <v>1.347219358530748</v>
       </c>
       <c r="AJ88">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="AK88" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="89" spans="1:37">
@@ -10624,10 +10624,10 @@
         <v>0.7176350047203662</v>
       </c>
       <c r="AJ91">
+        <v>2</v>
+      </c>
+      <c r="AK91" t="s">
         <v>6</v>
-      </c>
-      <c r="AK91" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="92" spans="1:37">
@@ -11171,10 +11171,10 @@
         <v>1.126665823732581</v>
       </c>
       <c r="AJ96">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="AK96" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
     </row>
     <row r="97" spans="1:37">
@@ -11831,10 +11831,10 @@
         <v>0.6546536707079771</v>
       </c>
       <c r="AJ102">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="AK102" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="103" spans="1:37">
@@ -12265,10 +12265,10 @@
         <v>0.7559289460184544</v>
       </c>
       <c r="AJ106">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="AK106" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="107" spans="1:37">
@@ -15976,10 +15976,10 @@
         <v>1.069044967649698</v>
       </c>
       <c r="AJ139">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="AK139" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
     </row>
     <row r="140" spans="1:37">
@@ -17653,10 +17653,10 @@
         <v>0.9639946650711892</v>
       </c>
       <c r="AJ154">
+        <v>2</v>
+      </c>
+      <c r="AK154" t="s">
         <v>6</v>
-      </c>
-      <c r="AK154" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="155" spans="1:37">
@@ -17748,10 +17748,10 @@
         <v>1.511857892036909</v>
       </c>
       <c r="AJ155">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="AK155" t="s">
-        <v>18</v>
+        <v>0</v>
       </c>
     </row>
     <row r="156" spans="1:37">
@@ -21007,10 +21007,10 @@
         <v>1.133893419027682</v>
       </c>
       <c r="AJ184">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="AK184" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
     </row>
     <row r="185" spans="1:37">
@@ -21328,10 +21328,10 @@
         <v>0.9108473292176121</v>
       </c>
       <c r="AJ187">
+        <v>2</v>
+      </c>
+      <c r="AK187" t="s">
         <v>6</v>
-      </c>
-      <c r="AK187" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="188" spans="1:37">
@@ -24587,10 +24587,10 @@
         <v>0.9488715101936315</v>
       </c>
       <c r="AJ216">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="AK216" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="217" spans="1:37">
@@ -25360,10 +25360,10 @@
         <v>0.8022290374770964</v>
       </c>
       <c r="AJ223">
+        <v>2</v>
+      </c>
+      <c r="AK223" t="s">
         <v>6</v>
-      </c>
-      <c r="AK223" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="224" spans="1:37">
@@ -28506,10 +28506,10 @@
         <v>0.7559289460184544</v>
       </c>
       <c r="AJ251">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="AK251" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
     </row>
     <row r="252" spans="1:37">
@@ -29957,10 +29957,10 @@
         <v>0.9788842044462081</v>
       </c>
       <c r="AJ264">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="AK264" t="s">
-        <v>18</v>
+        <v>0</v>
       </c>
     </row>
     <row r="265" spans="1:37">
@@ -32086,10 +32086,10 @@
         <v>0.3779644730092272</v>
       </c>
       <c r="AJ283">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="AK283" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
     </row>
     <row r="284" spans="1:37">
@@ -34102,10 +34102,10 @@
         <v>0.5345224838248488</v>
       </c>
       <c r="AJ301">
+        <v>2</v>
+      </c>
+      <c r="AK301" t="s">
         <v>6</v>
-      </c>
-      <c r="AK301" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="302" spans="1:37">
@@ -35214,10 +35214,10 @@
         <v>0.560930349636082</v>
       </c>
       <c r="AJ311">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="AK311" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="312" spans="1:37">
@@ -36665,10 +36665,10 @@
         <v>0.6546536707079771</v>
       </c>
       <c r="AJ324">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="AK324" t="s">
-        <v>18</v>
+        <v>0</v>
       </c>
     </row>
     <row r="325" spans="1:37">
@@ -36873,10 +36873,10 @@
         <v>0.5345224838248488</v>
       </c>
       <c r="AJ326">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="AK326" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
     </row>
     <row r="327" spans="1:37">
@@ -36968,10 +36968,10 @@
         <v>0.560930349636082</v>
       </c>
       <c r="AJ327">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="AK327" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
     </row>
     <row r="328" spans="1:37">
@@ -39971,10 +39971,10 @@
         <v>2.400849032058559</v>
       </c>
       <c r="AJ354">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AK354" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
     </row>
     <row r="355" spans="1:37">
@@ -40048,10 +40048,10 @@
         <v>1</v>
       </c>
       <c r="AJ355">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AK355" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="356" spans="1:37">
@@ -40125,10 +40125,10 @@
         <v>2.522712917791631</v>
       </c>
       <c r="AJ356">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AK356" t="s">
-        <v>0</v>
+        <v>24</v>
       </c>
     </row>
     <row r="357" spans="1:37">
@@ -40202,10 +40202,10 @@
         <v>3.295017884191656</v>
       </c>
       <c r="AJ357">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AK357" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="358" spans="1:37">
@@ -40279,10 +40279,10 @@
         <v>0.6546536707079771</v>
       </c>
       <c r="AJ358">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AK358" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="359" spans="1:37">
@@ -40356,10 +40356,10 @@
         <v>2.494465147626764</v>
       </c>
       <c r="AJ359">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AK359" t="s">
-        <v>0</v>
+        <v>24</v>
       </c>
     </row>
     <row r="360" spans="1:37">
@@ -40433,10 +40433,10 @@
         <v>2.425154056718762</v>
       </c>
       <c r="AJ360">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AK360" t="s">
-        <v>0</v>
+        <v>24</v>
       </c>
     </row>
     <row r="361" spans="1:37">
@@ -40510,10 +40510,10 @@
         <v>2</v>
       </c>
       <c r="AJ361">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AK361" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="362" spans="1:37">
@@ -40587,10 +40587,10 @@
         <v>0.6583931470512132</v>
       </c>
       <c r="AJ362">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AK362" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
     </row>
     <row r="363" spans="1:37">
@@ -40664,10 +40664,10 @@
         <v>1.812653934349931</v>
       </c>
       <c r="AJ363">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AK363" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="364" spans="1:37">
@@ -40741,10 +40741,10 @@
         <v>2.737774590451356</v>
       </c>
       <c r="AJ364">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AK364" t="s">
-        <v>0</v>
+        <v>24</v>
       </c>
     </row>
     <row r="365" spans="1:37">
@@ -40818,10 +40818,10 @@
         <v>2.815057855330246</v>
       </c>
       <c r="AJ365">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AK365" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
     </row>
     <row r="366" spans="1:37">
@@ -40895,10 +40895,10 @@
         <v>1.163544201487124</v>
       </c>
       <c r="AJ366">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AK366" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
     </row>
     <row r="367" spans="1:37">
@@ -40972,10 +40972,10 @@
         <v>1.812653934349931</v>
       </c>
       <c r="AJ367">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AK367" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="368" spans="1:37">
@@ -41049,10 +41049,10 @@
         <v>1.765715403226135</v>
       </c>
       <c r="AJ368">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AK368" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
     </row>
     <row r="369" spans="1:37">
@@ -41126,10 +41126,10 @@
         <v>3.27215643006847</v>
       </c>
       <c r="AJ369">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AK369" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
     </row>
     <row r="370" spans="1:37">
@@ -41203,10 +41203,10 @@
         <v>10.56564263929332</v>
       </c>
       <c r="AJ370">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AK370" t="s">
-        <v>0</v>
+        <v>24</v>
       </c>
     </row>
     <row r="371" spans="1:37">
@@ -41262,10 +41262,10 @@
         <v>1.362770287738494</v>
       </c>
       <c r="AJ371">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AK371" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="372" spans="1:37">
@@ -41339,10 +41339,10 @@
         <v>1.812653934349931</v>
       </c>
       <c r="AJ372">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AK372" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="373" spans="1:37">
@@ -41416,10 +41416,10 @@
         <v>1.055515318572638</v>
       </c>
       <c r="AJ373">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AK373" t="s">
-        <v>0</v>
+        <v>24</v>
       </c>
     </row>
     <row r="374" spans="1:37">
@@ -41493,10 +41493,10 @@
         <v>0.9769551550364136</v>
       </c>
       <c r="AJ374">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AK374" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
     </row>
     <row r="375" spans="1:37">
@@ -41570,10 +41570,10 @@
         <v>1.032970285763132</v>
       </c>
       <c r="AJ375">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AK375" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
     </row>
     <row r="376" spans="1:37">
@@ -41647,10 +41647,10 @@
         <v>1</v>
       </c>
       <c r="AJ376">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AK376" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="377" spans="1:37">
@@ -41724,10 +41724,10 @@
         <v>1.362770287738494</v>
       </c>
       <c r="AJ377">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AK377" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="378" spans="1:37">
@@ -41801,10 +41801,10 @@
         <v>5.365414951149214</v>
       </c>
       <c r="AJ378">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AK378" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
     </row>
     <row r="379" spans="1:37">
@@ -41878,10 +41878,10 @@
         <v>1.96641120786363</v>
       </c>
       <c r="AJ379">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AK379" t="s">
-        <v>0</v>
+        <v>24</v>
       </c>
     </row>
     <row r="380" spans="1:37">
@@ -41955,10 +41955,10 @@
         <v>2.721783580267223</v>
       </c>
       <c r="AJ380">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AK380" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="381" spans="1:37">
@@ -42026,10 +42026,10 @@
         <v>0.8451542547285166</v>
       </c>
       <c r="AJ381">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AK381" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="382" spans="1:37">
@@ -42103,10 +42103,10 @@
         <v>5.420804681439066</v>
       </c>
       <c r="AJ382">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AK382" t="s">
-        <v>0</v>
+        <v>21</v>
       </c>
     </row>
     <row r="383" spans="1:37">
@@ -42180,10 +42180,10 @@
         <v>1.935299451290558</v>
       </c>
       <c r="AJ383">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AK383" t="s">
-        <v>0</v>
+        <v>24</v>
       </c>
     </row>
     <row r="384" spans="1:37">
@@ -42257,10 +42257,10 @@
         <v>1.76477774090475</v>
       </c>
       <c r="AJ384">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AK384" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="385" spans="1:37">
@@ -42334,10 +42334,10 @@
         <v>3.31691906350497</v>
       </c>
       <c r="AJ385">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AK385" t="s">
-        <v>0</v>
+        <v>24</v>
       </c>
     </row>
     <row r="386" spans="1:37">
@@ -42411,10 +42411,10 @@
         <v>1.812452100251118</v>
       </c>
       <c r="AJ386">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AK386" t="s">
-        <v>0</v>
+        <v>24</v>
       </c>
     </row>
     <row r="387" spans="1:37">
@@ -42470,10 +42470,10 @@
         <v>2.699206232527312</v>
       </c>
       <c r="AJ387">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AK387" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="388" spans="1:37">
@@ -42547,10 +42547,10 @@
         <v>1.309307341415954</v>
       </c>
       <c r="AJ388">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AK388" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="389" spans="1:37">
@@ -42624,10 +42624,10 @@
         <v>2</v>
       </c>
       <c r="AJ389">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AK389" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="390" spans="1:37">
@@ -42701,10 +42701,10 @@
         <v>0.8561615991302028</v>
       </c>
       <c r="AJ390">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AK390" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
     </row>
     <row r="391" spans="1:37">
@@ -42778,10 +42778,10 @@
         <v>1.851640199545103</v>
       </c>
       <c r="AJ391">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AK391" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="392" spans="1:37">
@@ -42855,10 +42855,10 @@
         <v>1.647508942095828</v>
       </c>
       <c r="AJ392">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AK392" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="393" spans="1:37">
@@ -42932,10 +42932,10 @@
         <v>2.031749980748841</v>
       </c>
       <c r="AJ393">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AK393" t="s">
-        <v>0</v>
+        <v>24</v>
       </c>
     </row>
     <row r="394" spans="1:37">
@@ -43009,10 +43009,10 @@
         <v>1.069044967649698</v>
       </c>
       <c r="AJ394">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AK394" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="395" spans="1:37">
@@ -43086,10 +43086,10 @@
         <v>2.694361824427119</v>
       </c>
       <c r="AJ395">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AK395" t="s">
-        <v>0</v>
+        <v>24</v>
       </c>
     </row>
     <row r="396" spans="1:37">
@@ -43163,10 +43163,10 @@
         <v>2.381191714053275</v>
       </c>
       <c r="AJ396">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AK396" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="397" spans="1:37">
@@ -43240,10 +43240,10 @@
         <v>2.29906813420444</v>
       </c>
       <c r="AJ397">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AK397" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="398" spans="1:37">
@@ -43317,10 +43317,10 @@
         <v>1.216904503147478</v>
       </c>
       <c r="AJ398">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AK398" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
     </row>
     <row r="399" spans="1:37">
@@ -43394,10 +43394,10 @@
         <v>1.532872756844495</v>
       </c>
       <c r="AJ399">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AK399" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="400" spans="1:37">
@@ -43471,10 +43471,10 @@
         <v>1.549468314399042</v>
       </c>
       <c r="AJ400">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AK400" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
     </row>
     <row r="401" spans="1:37">
@@ -43548,10 +43548,10 @@
         <v>7.524478698574538</v>
       </c>
       <c r="AJ401">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AK401" t="s">
-        <v>0</v>
+        <v>24</v>
       </c>
     </row>
     <row r="402" spans="1:37">
@@ -43607,10 +43607,10 @@
         <v>1.927248223318863</v>
       </c>
       <c r="AJ402">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AK402" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="403" spans="1:37">
@@ -43684,10 +43684,10 @@
         <v>0.6546536707079771</v>
       </c>
       <c r="AJ403">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AK403" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="404" spans="1:37">
@@ -43761,10 +43761,10 @@
         <v>2.390457218668787</v>
       </c>
       <c r="AJ404">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AK404" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="405" spans="1:37">
@@ -43838,10 +43838,10 @@
         <v>0.9258200997725514</v>
       </c>
       <c r="AJ405">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AK405" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="406" spans="1:37">
@@ -43915,10 +43915,10 @@
         <v>3.964124835860459</v>
       </c>
       <c r="AJ406">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AK406" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="407" spans="1:37">
@@ -43992,10 +43992,10 @@
         <v>1.745859411713536</v>
       </c>
       <c r="AJ407">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AK407" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="408" spans="1:37">
@@ -44069,10 +44069,10 @@
         <v>2.420153478013916</v>
       </c>
       <c r="AJ408">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AK408" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="409" spans="1:37">
@@ -44146,10 +44146,10 @@
         <v>0.5897700009089515</v>
       </c>
       <c r="AJ409">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AK409" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="410" spans="1:37">
@@ -44223,10 +44223,10 @@
         <v>1.408958042747626</v>
       </c>
       <c r="AJ410">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AK410" t="s">
-        <v>0</v>
+        <v>24</v>
       </c>
     </row>
     <row r="411" spans="1:37">
@@ -44282,10 +44282,10 @@
         <v>2.449489742783178</v>
       </c>
       <c r="AJ411">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AK411" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="412" spans="1:37">
@@ -44359,10 +44359,10 @@
         <v>6.82416414269188</v>
       </c>
       <c r="AJ412">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AK412" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
     </row>
     <row r="413" spans="1:37">
@@ -44436,10 +44436,10 @@
         <v>3.16227766016838</v>
       </c>
       <c r="AJ413">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AK413" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="414" spans="1:37">
@@ -44513,10 +44513,10 @@
         <v>4.456135417280635</v>
       </c>
       <c r="AJ414">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AK414" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="415" spans="1:37">
@@ -44590,10 +44590,10 @@
         <v>2.449489742783178</v>
       </c>
       <c r="AJ415">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AK415" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="416" spans="1:37">
@@ -44667,10 +44667,10 @@
         <v>2.390457218668787</v>
       </c>
       <c r="AJ416">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AK416" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="417" spans="1:37">
@@ -44744,10 +44744,10 @@
         <v>2.410075808783777</v>
       </c>
       <c r="AJ417">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AK417" t="s">
-        <v>0</v>
+        <v>21</v>
       </c>
     </row>
     <row r="418" spans="1:37">
@@ -44821,10 +44821,10 @@
         <v>0.9258200997725514</v>
       </c>
       <c r="AJ418">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AK418" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="419" spans="1:37">
@@ -44898,10 +44898,10 @@
         <v>1.688100939904172</v>
       </c>
       <c r="AJ419">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AK419" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="420" spans="1:37">
@@ -44957,10 +44957,10 @@
         <v>0.7559289460184544</v>
       </c>
       <c r="AJ420">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AK420" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="421" spans="1:37">
@@ -45034,10 +45034,10 @@
         <v>2.463923226131743</v>
       </c>
       <c r="AJ421">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AK421" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="422" spans="1:37">
@@ -45111,10 +45111,10 @@
         <v>1.654077197484318</v>
       </c>
       <c r="AJ422">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AK422" t="s">
-        <v>0</v>
+        <v>24</v>
       </c>
     </row>
     <row r="423" spans="1:37">
@@ -45188,10 +45188,10 @@
         <v>1.520332431148054</v>
       </c>
       <c r="AJ423">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AK423" t="s">
-        <v>0</v>
+        <v>21</v>
       </c>
     </row>
     <row r="424" spans="1:37">
@@ -45265,10 +45265,10 @@
         <v>1.93001487987343</v>
       </c>
       <c r="AJ424">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AK424" t="s">
-        <v>0</v>
+        <v>24</v>
       </c>
     </row>
     <row r="425" spans="1:37">
@@ -45342,10 +45342,10 @@
         <v>2.47847879612821</v>
       </c>
       <c r="AJ425">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AK425" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="426" spans="1:37">
@@ -45419,10 +45419,10 @@
         <v>3.443420226626843</v>
       </c>
       <c r="AJ426">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AK426" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="427" spans="1:37">
@@ -45496,10 +45496,10 @@
         <v>2.138089935299395</v>
       </c>
       <c r="AJ427">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AK427" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="428" spans="1:37">
@@ -45573,10 +45573,10 @@
         <v>0.9258200997725514</v>
       </c>
       <c r="AJ428">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AK428" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="429" spans="1:37">
@@ -45650,10 +45650,10 @@
         <v>1.457794692162274</v>
       </c>
       <c r="AJ429">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AK429" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
     </row>
     <row r="430" spans="1:37">
@@ -45727,10 +45727,10 @@
         <v>1.690308509457033</v>
       </c>
       <c r="AJ430">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AK430" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="431" spans="1:37">
@@ -45804,10 +45804,10 @@
         <v>2.786677961420119</v>
       </c>
       <c r="AJ431">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AK431" t="s">
-        <v>0</v>
+        <v>21</v>
       </c>
     </row>
     <row r="432" spans="1:37">
@@ -45881,10 +45881,10 @@
         <v>1.49209768838824</v>
       </c>
       <c r="AJ432">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AK432" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
     </row>
     <row r="433" spans="1:37">
@@ -45958,10 +45958,10 @@
         <v>4.049929573971514</v>
       </c>
       <c r="AJ433">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AK433" t="s">
-        <v>0</v>
+        <v>24</v>
       </c>
     </row>
     <row r="434" spans="1:37">
@@ -46017,10 +46017,10 @@
         <v>3.854496446637726</v>
       </c>
       <c r="AJ434">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AK434" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="435" spans="1:37">
@@ -46094,10 +46094,10 @@
         <v>2.29906813420444</v>
       </c>
       <c r="AJ435">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AK435" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="436" spans="1:37">
@@ -46171,10 +46171,10 @@
         <v>2.186035568629555</v>
       </c>
       <c r="AJ436">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AK436" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
     </row>
     <row r="437" spans="1:37">
@@ -46248,10 +46248,10 @@
         <v>2.706168802162738</v>
       </c>
       <c r="AJ437">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AK437" t="s">
-        <v>0</v>
+        <v>24</v>
       </c>
     </row>
     <row r="438" spans="1:37">
@@ -46325,10 +46325,10 @@
         <v>1.521111721636927</v>
       </c>
       <c r="AJ438">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AK438" t="s">
-        <v>0</v>
+        <v>21</v>
       </c>
     </row>
     <row r="439" spans="1:37">
@@ -46402,10 +46402,10 @@
         <v>5.028490259085155</v>
       </c>
       <c r="AJ439">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AK439" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="440" spans="1:37">
@@ -46479,10 +46479,10 @@
         <v>2.291418820735684</v>
       </c>
       <c r="AJ440">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AK440" t="s">
-        <v>0</v>
+        <v>24</v>
       </c>
     </row>
     <row r="441" spans="1:37">
@@ -46556,10 +46556,10 @@
         <v>4.342481186734475</v>
       </c>
       <c r="AJ441">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AK441" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="442" spans="1:37">
@@ -46633,10 +46633,10 @@
         <v>3.044819186089005</v>
       </c>
       <c r="AJ442">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AK442" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
     </row>
     <row r="443" spans="1:37">
@@ -46710,10 +46710,10 @@
         <v>2.938344377860274</v>
       </c>
       <c r="AJ443">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AK443" t="s">
-        <v>0</v>
+        <v>21</v>
       </c>
     </row>
     <row r="444" spans="1:37">
@@ -46787,10 +46787,10 @@
         <v>3.303766029604326</v>
       </c>
       <c r="AJ444">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AK444" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="445" spans="1:37">
@@ -46864,10 +46864,10 @@
         <v>2.420153478013916</v>
       </c>
       <c r="AJ445">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AK445" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="446" spans="1:37">
@@ -46941,10 +46941,10 @@
         <v>4.675162334843877</v>
       </c>
       <c r="AJ446">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AK446" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="447" spans="1:37">
@@ -47018,10 +47018,10 @@
         <v>1.602136011568684</v>
       </c>
       <c r="AJ447">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AK447" t="s">
-        <v>0</v>
+        <v>21</v>
       </c>
     </row>
     <row r="448" spans="1:37">
@@ -47095,10 +47095,10 @@
         <v>1.341192210821942</v>
       </c>
       <c r="AJ448">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AK448" t="s">
-        <v>0</v>
+        <v>24</v>
       </c>
     </row>
     <row r="449" spans="1:37">
@@ -47172,10 +47172,10 @@
         <v>3.019696049274081</v>
       </c>
       <c r="AJ449">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AK449" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
     </row>
     <row r="450" spans="1:37">
@@ -47249,10 +47249,10 @@
         <v>1.506579087598272</v>
       </c>
       <c r="AJ450">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AK450" t="s">
-        <v>0</v>
+        <v>21</v>
       </c>
     </row>
     <row r="451" spans="1:37">
@@ -47326,10 +47326,10 @@
         <v>6.90755280213519</v>
       </c>
       <c r="AJ451">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AK451" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="452" spans="1:37">
@@ -47403,10 +47403,10 @@
         <v>1.414213562373095</v>
       </c>
       <c r="AJ452">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AK452" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="453" spans="1:37">
@@ -47480,10 +47480,10 @@
         <v>1.844939014442558</v>
       </c>
       <c r="AJ453">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AK453" t="s">
-        <v>0</v>
+        <v>21</v>
       </c>
     </row>
     <row r="454" spans="1:37">
@@ -47557,10 +47557,10 @@
         <v>2.591193878173865</v>
       </c>
       <c r="AJ454">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AK454" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="455" spans="1:37">
@@ -47634,10 +47634,10 @@
         <v>0.6546536707079771</v>
       </c>
       <c r="AJ455">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AK455" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="456" spans="1:37">
@@ -47711,10 +47711,10 @@
         <v>2.803504543722369</v>
       </c>
       <c r="AJ456">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AK456" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
     </row>
     <row r="457" spans="1:37">
@@ -47788,10 +47788,10 @@
         <v>2.548572483249095</v>
       </c>
       <c r="AJ457">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AK457" t="s">
-        <v>0</v>
+        <v>24</v>
       </c>
     </row>
     <row r="458" spans="1:37">
@@ -47865,10 +47865,10 @@
         <v>2.795153197629088</v>
       </c>
       <c r="AJ458">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AK458" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
     </row>
     <row r="459" spans="1:37">
@@ -47942,10 +47942,10 @@
         <v>1.746628614787709</v>
       </c>
       <c r="AJ459">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AK459" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
     </row>
     <row r="460" spans="1:37">
@@ -48019,10 +48019,10 @@
         <v>2.893985122076367</v>
       </c>
       <c r="AJ460">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AK460" t="s">
-        <v>0</v>
+        <v>24</v>
       </c>
     </row>
     <row r="461" spans="1:37">
@@ -48096,10 +48096,10 @@
         <v>0.5345224838248488</v>
       </c>
       <c r="AJ461">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AK461" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="462" spans="1:37">
@@ -48173,10 +48173,10 @@
         <v>3</v>
       </c>
       <c r="AJ462">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AK462" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="463" spans="1:37">
@@ -48250,10 +48250,10 @@
         <v>2.751622897751175</v>
       </c>
       <c r="AJ463">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AK463" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="464" spans="1:37">
@@ -48327,10 +48327,10 @@
         <v>4.735881272643079</v>
       </c>
       <c r="AJ464">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AK464" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="465" spans="1:37">
@@ -48404,10 +48404,10 @@
         <v>2.752862451360901</v>
       </c>
       <c r="AJ465">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AK465" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
     </row>
     <row r="466" spans="1:37">
@@ -48481,10 +48481,10 @@
         <v>1.675428187015472</v>
       </c>
       <c r="AJ466">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AK466" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
     </row>
     <row r="467" spans="1:37">
@@ -48558,10 +48558,10 @@
         <v>2.212239980573742</v>
       </c>
       <c r="AJ467">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AK467" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
     </row>
     <row r="468" spans="1:37">
@@ -48635,10 +48635,10 @@
         <v>1.836699471225101</v>
       </c>
       <c r="AJ468">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AK468" t="s">
-        <v>0</v>
+        <v>21</v>
       </c>
     </row>
     <row r="469" spans="1:37">
@@ -48712,10 +48712,10 @@
         <v>1.309307341415954</v>
       </c>
       <c r="AJ469">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AK469" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="470" spans="1:37">
@@ -48789,10 +48789,10 @@
         <v>2.117344015212511</v>
       </c>
       <c r="AJ470">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AK470" t="s">
-        <v>0</v>
+        <v>24</v>
       </c>
     </row>
     <row r="471" spans="1:37">
@@ -48866,10 +48866,10 @@
         <v>1.732050807568877</v>
       </c>
       <c r="AJ471">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AK471" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="472" spans="1:37">
@@ -48943,10 +48943,10 @@
         <v>0.9258200997725514</v>
       </c>
       <c r="AJ472">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AK472" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="473" spans="1:37">
@@ -49020,10 +49020,10 @@
         <v>1.253566341056017</v>
       </c>
       <c r="AJ473">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AK473" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="474" spans="1:37">
@@ -49097,10 +49097,10 @@
         <v>1.309307341415954</v>
       </c>
       <c r="AJ474">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AK474" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="475" spans="1:37">
@@ -49174,10 +49174,10 @@
         <v>8.27358904995824</v>
       </c>
       <c r="AJ475">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AK475" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
     </row>
     <row r="476" spans="1:37">
@@ -49251,10 +49251,10 @@
         <v>4.325632796807265</v>
       </c>
       <c r="AJ476">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AK476" t="s">
-        <v>0</v>
+        <v>24</v>
       </c>
     </row>
     <row r="477" spans="1:37">
@@ -49328,10 +49328,10 @@
         <v>1.253566341056017</v>
       </c>
       <c r="AJ477">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AK477" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="478" spans="1:37">
@@ -49405,10 +49405,10 @@
         <v>2.232949852414325</v>
       </c>
       <c r="AJ478">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AK478" t="s">
-        <v>0</v>
+        <v>24</v>
       </c>
     </row>
     <row r="479" spans="1:37">
@@ -49482,10 +49482,10 @@
         <v>3.671467292918515</v>
       </c>
       <c r="AJ479">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AK479" t="s">
-        <v>0</v>
+        <v>24</v>
       </c>
     </row>
     <row r="480" spans="1:37">
@@ -49559,10 +49559,10 @@
         <v>0.9258200997725514</v>
       </c>
       <c r="AJ480">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AK480" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="481" spans="1:37">
@@ -49636,10 +49636,10 @@
         <v>6.970283542441617</v>
       </c>
       <c r="AJ481">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AK481" t="s">
-        <v>0</v>
+        <v>24</v>
       </c>
     </row>
     <row r="482" spans="1:37">
@@ -49713,10 +49713,10 @@
         <v>1.927248223318863</v>
       </c>
       <c r="AJ482">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AK482" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="483" spans="1:37">
@@ -49772,10 +49772,10 @@
         <v>2.449489742783178</v>
       </c>
       <c r="AJ483">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AK483" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="484" spans="1:37">
@@ -49849,10 +49849,10 @@
         <v>2.23122775853075</v>
       </c>
       <c r="AJ484">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AK484" t="s">
-        <v>0</v>
+        <v>21</v>
       </c>
     </row>
     <row r="485" spans="1:37">
@@ -49926,10 +49926,10 @@
         <v>1.341825175593519</v>
       </c>
       <c r="AJ485">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AK485" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
     </row>
     <row r="486" spans="1:37">
@@ -50003,10 +50003,10 @@
         <v>1.232865739455297</v>
       </c>
       <c r="AJ486">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AK486" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
     </row>
     <row r="487" spans="1:37">
@@ -50080,10 +50080,10 @@
         <v>1.922132804047698</v>
       </c>
       <c r="AJ487">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AK487" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
     </row>
     <row r="488" spans="1:37">
@@ -50139,10 +50139,10 @@
         <v>2.618614682831908</v>
       </c>
       <c r="AJ488">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AK488" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="489" spans="1:37">
@@ -50216,10 +50216,10 @@
         <v>1.511857892036909</v>
       </c>
       <c r="AJ489">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AK489" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="490" spans="1:37">
@@ -50293,10 +50293,10 @@
         <v>0.5107427474637944</v>
       </c>
       <c r="AJ490">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AK490" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
     </row>
     <row r="491" spans="1:37">
@@ -50370,10 +50370,10 @@
         <v>4.791509786565817</v>
       </c>
       <c r="AJ491">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AK491" t="s">
-        <v>0</v>
+        <v>21</v>
       </c>
     </row>
     <row r="492" spans="1:37">
@@ -50429,10 +50429,10 @@
         <v>3.229329872987805</v>
       </c>
       <c r="AJ492">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AK492" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="493" spans="1:37">
@@ -50506,10 +50506,10 @@
         <v>3.093772546815388</v>
       </c>
       <c r="AJ493">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AK493" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="494" spans="1:37">
@@ -50583,10 +50583,10 @@
         <v>5.928141120356123</v>
       </c>
       <c r="AJ494">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AK494" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="495" spans="1:37">
@@ -50660,10 +50660,10 @@
         <v>1.647508942095828</v>
       </c>
       <c r="AJ495">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AK495" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="496" spans="1:37">
@@ -50737,10 +50737,10 @@
         <v>18.55108776171514</v>
       </c>
       <c r="AJ496">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AK496" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="497" spans="1:37">
@@ -50814,10 +50814,10 @@
         <v>2.354603014959224</v>
       </c>
       <c r="AJ497">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AK497" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="498" spans="1:37">
@@ -50891,10 +50891,10 @@
         <v>2.699206232527312</v>
       </c>
       <c r="AJ498">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AK498" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="499" spans="1:37">
@@ -50968,10 +50968,10 @@
         <v>2.212192496312944</v>
       </c>
       <c r="AJ499">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AK499" t="s">
-        <v>0</v>
+        <v>24</v>
       </c>
     </row>
     <row r="500" spans="1:37">
@@ -51045,10 +51045,10 @@
         <v>0.809030804158977</v>
       </c>
       <c r="AJ500">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AK500" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
     </row>
     <row r="501" spans="1:37">
@@ -51122,10 +51122,10 @@
         <v>4.332557214890089</v>
       </c>
       <c r="AJ501">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AK501" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
     </row>
     <row r="502" spans="1:37">
@@ -51199,10 +51199,10 @@
         <v>0.9258200997725514</v>
       </c>
       <c r="AJ502">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AK502" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="503" spans="1:37">
@@ -51258,10 +51258,10 @@
         <v>6.233549779791836</v>
       </c>
       <c r="AJ503">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AK503" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="504" spans="1:37">
@@ -51335,10 +51335,10 @@
         <v>1.772810520855837</v>
       </c>
       <c r="AJ504">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AK504" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="505" spans="1:37">
@@ -51412,10 +51412,10 @@
         <v>1.362770287738494</v>
       </c>
       <c r="AJ505">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AK505" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="506" spans="1:37">
@@ -51471,10 +51471,10 @@
         <v>1.268523948167463</v>
       </c>
       <c r="AJ506">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AK506" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="507" spans="1:37">
@@ -51548,10 +51548,10 @@
         <v>1.2321906164089</v>
       </c>
       <c r="AJ507">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AK507" t="s">
-        <v>0</v>
+        <v>21</v>
       </c>
     </row>
     <row r="508" spans="1:37">
@@ -51625,10 +51625,10 @@
         <v>3.959961557580163</v>
       </c>
       <c r="AJ508">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AK508" t="s">
-        <v>0</v>
+        <v>21</v>
       </c>
     </row>
     <row r="509" spans="1:37">
@@ -51702,10 +51702,10 @@
         <v>1.989908477333977</v>
       </c>
       <c r="AJ509">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AK509" t="s">
-        <v>0</v>
+        <v>24</v>
       </c>
     </row>
     <row r="510" spans="1:37">
@@ -51779,10 +51779,10 @@
         <v>86.0720578498737</v>
       </c>
       <c r="AJ510">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AK510" t="s">
-        <v>0</v>
+        <v>24</v>
       </c>
     </row>
     <row r="511" spans="1:37">
@@ -51856,10 +51856,10 @@
         <v>2.303826940470526</v>
       </c>
       <c r="AJ511">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AK511" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
     </row>
     <row r="512" spans="1:37">
@@ -51933,10 +51933,10 @@
         <v>2.237245226735704</v>
       </c>
       <c r="AJ512">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AK512" t="s">
-        <v>0</v>
+        <v>24</v>
       </c>
     </row>
     <row r="513" spans="1:37">
@@ -52010,10 +52010,10 @@
         <v>4.58257569495584</v>
       </c>
       <c r="AJ513">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AK513" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="514" spans="1:37">
@@ -52087,10 +52087,10 @@
         <v>1.461379987405658</v>
       </c>
       <c r="AJ514">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AK514" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
     </row>
     <row r="515" spans="1:37">
@@ -52164,10 +52164,10 @@
         <v>0.5345224838248488</v>
       </c>
       <c r="AJ515">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AK515" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="516" spans="1:37">
@@ -52241,10 +52241,10 @@
         <v>1.4638501094228</v>
       </c>
       <c r="AJ516">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AK516" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="517" spans="1:37">
@@ -52318,10 +52318,10 @@
         <v>6.556914747000878</v>
       </c>
       <c r="AJ517">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AK517" t="s">
-        <v>0</v>
+        <v>21</v>
       </c>
     </row>
     <row r="518" spans="1:37">
@@ -52395,10 +52395,10 @@
         <v>1.690308509457033</v>
       </c>
       <c r="AJ518">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AK518" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="519" spans="1:37">
@@ -52472,10 +52472,10 @@
         <v>2.796100577452149</v>
       </c>
       <c r="AJ519">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AK519" t="s">
-        <v>0</v>
+        <v>24</v>
       </c>
     </row>
     <row r="520" spans="1:37">
@@ -52549,10 +52549,10 @@
         <v>1.927248223318863</v>
       </c>
       <c r="AJ520">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AK520" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="521" spans="1:37">
@@ -52608,10 +52608,10 @@
         <v>2.9277002188456</v>
       </c>
       <c r="AJ521">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AK521" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="522" spans="1:37">
@@ -52685,10 +52685,10 @@
         <v>1.069044967649698</v>
       </c>
       <c r="AJ522">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AK522" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="523" spans="1:37">
@@ -52762,10 +52762,10 @@
         <v>1.647508942095828</v>
       </c>
       <c r="AJ523">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AK523" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="524" spans="1:37">
@@ -52839,10 +52839,10 @@
         <v>2.071470402166487</v>
       </c>
       <c r="AJ524">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AK524" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
     </row>
     <row r="525" spans="1:37">
@@ -52916,10 +52916,10 @@
         <v>2.759322168548819</v>
       </c>
       <c r="AJ525">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AK525" t="s">
-        <v>0</v>
+        <v>24</v>
       </c>
     </row>
     <row r="526" spans="1:37">
@@ -52993,10 +52993,10 @@
         <v>12.96148139681572</v>
       </c>
       <c r="AJ526">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AK526" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="527" spans="1:37">
@@ -53070,10 +53070,10 @@
         <v>1.395921178034278</v>
       </c>
       <c r="AJ527">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AK527" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="528" spans="1:37">
@@ -53147,10 +53147,10 @@
         <v>0.5345224838248488</v>
       </c>
       <c r="AJ528">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AK528" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="529" spans="1:37">
@@ -53224,10 +53224,10 @@
         <v>3.039274625611673</v>
       </c>
       <c r="AJ529">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AK529" t="s">
-        <v>0</v>
+        <v>24</v>
       </c>
     </row>
     <row r="530" spans="1:37">
@@ -53301,10 +53301,10 @@
         <v>1.412839042529799</v>
       </c>
       <c r="AJ530">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AK530" t="s">
-        <v>0</v>
+        <v>24</v>
       </c>
     </row>
     <row r="531" spans="1:37">
@@ -53378,10 +53378,10 @@
         <v>2.751622897751175</v>
       </c>
       <c r="AJ531">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AK531" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="532" spans="1:37">
@@ -53455,10 +53455,10 @@
         <v>2.152026379039378</v>
       </c>
       <c r="AJ532">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AK532" t="s">
-        <v>0</v>
+        <v>21</v>
       </c>
     </row>
     <row r="533" spans="1:37">
@@ -53532,10 +53532,10 @@
         <v>3.236942850933003</v>
       </c>
       <c r="AJ533">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AK533" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
     </row>
     <row r="534" spans="1:37">
@@ -53609,10 +53609,10 @@
         <v>2.448121076239397</v>
       </c>
       <c r="AJ534">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AK534" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
     </row>
     <row r="535" spans="1:37">
@@ -53686,10 +53686,10 @@
         <v>3.240379963422582</v>
       </c>
       <c r="AJ535">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AK535" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
     </row>
     <row r="536" spans="1:37">
@@ -53763,10 +53763,10 @@
         <v>2.023478345610805</v>
       </c>
       <c r="AJ536">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AK536" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="537" spans="1:37">
@@ -53840,10 +53840,10 @@
         <v>2.332069007896982</v>
       </c>
       <c r="AJ537">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AK537" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="538" spans="1:37">
@@ -53899,10 +53899,10 @@
         <v>21.7836804909735</v>
       </c>
       <c r="AJ538">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AK538" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="539" spans="1:37">
@@ -53976,10 +53976,10 @@
         <v>1.137873142435542</v>
       </c>
       <c r="AJ539">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AK539" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
     </row>
     <row r="540" spans="1:37">
@@ -54053,10 +54053,10 @@
         <v>7.473763634016188</v>
       </c>
       <c r="AJ540">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AK540" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="541" spans="1:37">
@@ -54112,10 +54112,10 @@
         <v>30.46074757548053</v>
       </c>
       <c r="AJ541">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AK541" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="542" spans="1:37">
@@ -54189,10 +54189,10 @@
         <v>1.069044967649698</v>
       </c>
       <c r="AJ542">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AK542" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="543" spans="1:37">
@@ -54266,10 +54266,10 @@
         <v>3.207134902949093</v>
       </c>
       <c r="AJ543">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AK543" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="544" spans="1:37">
@@ -54325,10 +54325,10 @@
         <v>0.5345224838248488</v>
       </c>
       <c r="AJ544">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AK544" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="545" spans="1:37">
@@ -54384,10 +54384,10 @@
         <v>2.507132682112035</v>
       </c>
       <c r="AJ545">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AK545" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="546" spans="1:37">
@@ -54461,10 +54461,10 @@
         <v>1.253566341056017</v>
       </c>
       <c r="AJ546">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AK546" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>